<commit_message>
add utils.py and revision main
</commit_message>
<xml_diff>
--- a/asset/Simplified Hierachical Table.xlsx
+++ b/asset/Simplified Hierachical Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学习\Tabular QA\Table数据集\HiTab\data\tables\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学习\Tabular QA\工作内容\Table Transformation\Table-Transformation-demo\asset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD257A01-6152-4E0A-A930-91F2AC90D019}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28503034-C452-49D4-BF1E-4095CB4B0806}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="12045" windowHeight="4980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -636,6 +636,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -765,7 +846,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -787,17 +868,32 @@
     <xf numFmtId="0" fontId="19" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1157,7 +1253,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1171,24 +1267,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="10"/>
+      <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="7">
+      <c r="C1" s="8">
         <v>2018</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8">
         <v>2019</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1215,7 +1311,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1247,7 +1343,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1260,7 +1356,7 @@
       <c r="E4" s="4">
         <v>11.3</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>13.3</v>
       </c>
       <c r="G4" s="4">
@@ -1277,7 +1373,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1403,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1337,7 +1433,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1367,7 +1463,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1493,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1429,7 +1525,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1442,7 +1538,7 @@
       <c r="E10" s="4">
         <v>10.8</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>14.6</v>
       </c>
       <c r="G10" s="4">
@@ -1459,7 +1555,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1585,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1519,7 +1615,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1549,7 +1645,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1579,11 +1675,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>